<commit_message>
Updated by Bot-Parser on 2023-03-23T16:42:19+00:00
</commit_message>
<xml_diff>
--- a/cves.xlsx
+++ b/cves.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D179"/>
+  <dimension ref="A1:D174"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -598,7 +598,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CVE-2023-26544</t>
+          <t>CVE-2023-28339</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -606,19 +606,19 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>In the Linux kernel 6.0.8, there is a use-after-free in run_unpack in fs/ntfs3/run.c, related to a difference between NTFS sector size and media sector size.</t>
+          <t>OpenDoas through 6.8.2, when TIOCSTI is available, allows privilege escalation because of sharing a terminal with the original session. NOTE: TIOCSTI is unavailable in OpenBSD 6.0 and later, and can be made unavailable in the Linux kernel 6.2 and later.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2023-03-16T16:15:12.087</t>
+          <t>2023-03-21T14:04:38.757</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CVE-2023-26545</t>
+          <t>CVE-2023-28466</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -626,52 +626,52 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>In the Linux kernel before 6.1.13, there is a double free in net/mpls/af_mpls.c upon an allocation failure (for registering the sysctl table under a new location) during the renaming of a device.</t>
+          <t>do_tls_getsockopt in net/tls/tls_main.c in the Linux kernel through 6.2.6 lacks a lock_sock call, leading to a race condition (with a resultant use-after-free or NULL pointer dereference).</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2023-03-16T16:15:12.167</t>
+          <t>2023-03-21T17:27:19.377</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CVE-2023-26605</t>
+          <t>CVE-2023-28100</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>5.9</v>
+        <v>6</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>In the Linux kernel 6.0.8, there is a use-after-free in inode_cgwb_move_to_attached in fs/fs-writeback.c, related to __list_del_entry_valid.</t>
+          <t>Flatpak is a system for building, distributing, and running sandboxed desktop applications on Linux. Versions prior to 1.10.8, 1.12.8, 1.14.4, and 1.15.4 contain a vulnerability similar to CVE-2017-5226, but using the `TIOCLINUX` ioctl command instead of `TIOCSTI`. If a Flatpak app is run on a Linux virtual console such as `/dev/tty1`, it can copy text from the virtual console and paste it into the command buffer, from which the command might be run after the Flatpak app has exited. Ordinary graphical terminal emulators like xterm, gnome-terminal and Konsole are unaffected. This vulnerability is specific to the Linux virtual consoles `/dev/tty1`, `/dev/tty2` and so on. A patch is available in versions 1.10.8, 1.12.8, 1.14.4, and 1.15.4. As a workaround, don't run Flatpak on a Linux virtual console. Flatpak is primarily designed to be used in a Wayland or X11 graphical environment.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2023-03-16T16:15:12.247</t>
+          <t>2023-03-22T19:13:43.267</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CVE-2023-26606</t>
+          <t>CVE-2023-28101</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>5.9</v>
+        <v>1.4</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>In the Linux kernel 6.0.8, there is a use-after-free in ntfs_trim_fs in fs/ntfs3/bitmap.c.</t>
+          <t>Flatpak is a system for building, distributing, and running sandboxed desktop applications on Linux. In versions prior to 1.10.8, 1.12.8, 1.14.4, and 1.15.4, if an attacker publishes a Flatpak app with elevated permissions, they can hide those permissions from users of the `flatpak(1)` command-line interface by setting other permissions to crafted values that contain non-printable control characters such as `ESC`. A fix is available in versions 1.10.8, 1.12.8, 1.14.4, and 1.15.4. As a workaround, use a GUI like GNOME Software rather than the command-line interface, or only install apps whose maintainers you trust.</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2023-03-16T16:15:12.323</t>
+          <t>2023-03-22T19:02:43.367</t>
         </is>
       </c>
     </row>
@@ -1734,67 +1734,67 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>CVE-2023-24580</t>
+          <t>CVE-2023-26075</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>3.6</v>
+        <v>5.9</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>An issue was discovered in the Multipart Request Parser in Django 3.2 before 3.2.18, 4.0 before 4.0.10, and 4.1 before 4.1.7. Passing certain inputs (e.g., an excessive number of parts) to multipart forms could result in too many open files or memory exhaustion, and provided a potential vector for a denial-of-service attack.</t>
+          <t>An issue was discovered in Samsung Mobile Chipset and Baseband Modem Chipset for Exynos 850, Exynos 980, Exynos 1080, Exynos 1280, Exynos 2200, Exynos Modem 5123, Exynos Modem 5300, and Exynos Auto T5123. An intra-object overflow in the 5G MM message codec can occur due to insufficient parameter validation when decoding the Service Area List.</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>2023-03-16T16:15:11.990</t>
+          <t>2023-03-17T16:15:11.950</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>CVE-2023-26075</t>
+          <t>CVE-2023-1369</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>5.9</v>
+        <v>3.6</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>An issue was discovered in Samsung Mobile Chipset and Baseband Modem Chipset for Exynos 850, Exynos 980, Exynos 1080, Exynos 1280, Exynos 2200, Exynos Modem 5123, Exynos Modem 5300, and Exynos Auto T5123. An intra-object overflow in the 5G MM message codec can occur due to insufficient parameter validation when decoding the Service Area List.</t>
+          <t>A vulnerability was found in TG Soft Vir.IT eXplorer 9.4.86.0. It has been rated as problematic. This issue affects some unknown processing in the library VIRAGTLT.sys of the component IoControlCode Handler. The manipulation leads to denial of service. The attack needs to be approached locally. The exploit has been disclosed to the public and may be used. Upgrading to version 9.5 is able to address this issue. It is recommended to upgrade the affected component. The associated identifier of this vulnerability is VDB-222875.</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>2023-03-17T16:15:11.950</t>
+          <t>2023-03-17T14:23:27.827</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>CVE-2023-1369</t>
+          <t>CVE-2023-26072</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>3.6</v>
+        <v>5.9</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>A vulnerability was found in TG Soft Vir.IT eXplorer 9.4.86.0. It has been rated as problematic. This issue affects some unknown processing in the library VIRAGTLT.sys of the component IoControlCode Handler. The manipulation leads to denial of service. The attack needs to be approached locally. The exploit has been disclosed to the public and may be used. Upgrading to version 9.5 is able to address this issue. It is recommended to upgrade the affected component. The associated identifier of this vulnerability is VDB-222875.</t>
+          <t>An issue was discovered in Samsung Mobile Chipset and Baseband Modem Chipset for Exynos 850, Exynos 980, Exynos 1080, Exynos 1280, Exynos 2200, Exynos Modem 5123, Exynos Modem 5300, and Exynos Auto T5123. A heap-based buffer overflow in the 5G MM message codec can occur due to insufficient parameter validation when decoding the Emergency number list.</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2023-03-17T14:23:27.827</t>
+          <t>2023-03-17T16:15:11.517</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>CVE-2023-26072</t>
+          <t>CVE-2023-26074</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1802,12 +1802,12 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>An issue was discovered in Samsung Mobile Chipset and Baseband Modem Chipset for Exynos 850, Exynos 980, Exynos 1080, Exynos 1280, Exynos 2200, Exynos Modem 5123, Exynos Modem 5300, and Exynos Auto T5123. A heap-based buffer overflow in the 5G MM message codec can occur due to insufficient parameter validation when decoding the Emergency number list.</t>
+          <t>An issue was discovered in Samsung Mobile Chipset and Baseband Modem Chipset for Exynos 850, Exynos 980, Exynos 1080, Exynos 1280, Exynos 2200, Exynos Modem 5123, Exynos Modem 5300, and Exynos Auto T5123.. A heap-based buffer overflow in the 5G MM message codec can occur due to insufficient parameter validation when decoding operator-defined access category definitions.</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2023-03-17T16:15:11.517</t>
+          <t>2023-03-17T16:15:11.780</t>
         </is>
       </c>
     </row>
@@ -1914,7 +1914,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>CVE-2023-0795</t>
+          <t>CVE-2023-0361</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -1922,19 +1922,19 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>LibTIFF 4.4.0 has an out-of-bounds read in tiffcrop in tools/tiffcrop.c:3488, allowing attackers to cause a denial-of-service via a crafted tiff file. For users that compile libtiff from sources, the fix is available with commit afaabc3e.</t>
+          <t>A timing side-channel in the handling of RSA ClientKeyExchange messages was discovered in GnuTLS. This side-channel can be sufficient to recover the key encrypted in the RSA ciphertext across a network in a Bleichenbacher style attack. To achieve a successful decryption the attacker would need to send a large amount of specially crafted messages to the vulnerable server. By recovering the secret from the ClientKeyExchange message, the attacker would be able to decrypt the application data exchanged over that connection.</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>2023-03-16T16:15:11.000</t>
+          <t>2023-03-18T07:15:10.870</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>CVE-2023-0796</t>
+          <t>CVE-2022-4645</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -1942,39 +1942,39 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>LibTIFF 4.4.0 has an out-of-bounds read in tiffcrop in tools/tiffcrop.c:3592, allowing attackers to cause a denial-of-service via a crafted tiff file. For users that compile libtiff from sources, the fix is available with commit afaabc3e.</t>
+          <t>LibTIFF 4.4.0 has an out-of-bounds read in tiffcp in tools/tiffcp.c:948, allowing attackers to cause a denial-of-service via a crafted tiff file. For users that compile libtiff from sources, the fix is available with commit e8131125.</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>2023-03-16T16:15:11.107</t>
+          <t>2023-03-16T20:15:11.220</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>CVE-2023-0798</t>
+          <t>CVE-2023-1161</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>3.6</v>
+        <v>4.2</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>LibTIFF 4.4.0 has an out-of-bounds read in tiffcrop in tools/tiffcrop.c:3400, allowing attackers to cause a denial-of-service via a crafted tiff file. For users that compile libtiff from sources, the fix is available with commit afaabc3e.</t>
+          <t>ISO 15765 and ISO 10681 dissector crash in Wireshark 4.0.0 to 4.0.3 and 3.6.0 to 3.6.11 allows denial of service via packet injection or crafted capture file</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>2023-03-16T16:15:11.187</t>
+          <t>2023-03-21T16:21:10.957</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>CVE-2023-0799</t>
+          <t>CVE-2022-4315</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -1982,12 +1982,12 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>LibTIFF 4.4.0 has an out-of-bounds read in tiffcrop in tools/tiffcrop.c:3701, allowing attackers to cause a denial-of-service via a crafted tiff file. For users that compile libtiff from sources, the fix is available with commit afaabc3e.</t>
+          <t>An issue has been discovered in GitLab DAST analyzer affecting all versions starting from 2.0 before 3.0.55, which sends custom request headers with every request on the authentication page.</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>2023-03-16T16:15:11.283</t>
+          <t>2023-03-22T14:15:15.990</t>
         </is>
       </c>
     </row>
@@ -2254,45 +2254,45 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>CVE-2023-23919</t>
-        </is>
-      </c>
-      <c r="B92" t="n">
-        <v>3.6</v>
-      </c>
+          <t>CVE-2023-0464</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr"/>
       <c r="C92" t="inlineStr">
         <is>
-          <t>A cryptographic vulnerability exists in Node.js &lt;19.2.0, &lt;18.14.1, &lt;16.19.1, &lt;14.21.3 that in some cases did does not clear the OpenSSL error stack after operations that may set it. This may lead to false positive errors during subsequent cryptographic operations that happen to be on the same thread. This in turn could be used to cause a denial of service.</t>
+          <t>A security vulnerability has been identified in all supported versions of OpenSSL related to the verification of X.509 certificate chains that include policy constraints. Attackers may be able to exploit this vulnerability by creating a malicious certificate chain that triggers exponential use of computational resources, leading to a denial-of-service (DoS) attack on affected systems. Policy processing is disabled by default but can be enabled by passing the `-policy' argument to the command line utilities or by calling the `X509_VERIFY_PARAM_set1_policies()' function.</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>2023-03-16T16:15:11.810</t>
+          <t>2023-03-22T18:10:33.697</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>CVE-2023-0464</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr"/>
+          <t>CVE-2021-24705</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>2.7</v>
+      </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>A security vulnerability has been identified in all supported versions of OpenSSL related to the verification of X.509 certificate chains that include policy constraints. Attackers may be able to exploit this vulnerability by creating a malicious certificate chain that triggers exponential use of computational resources, leading to a denial-of-service (DoS) attack on affected systems. Policy processing is disabled by default but can be enabled by passing the `-policy' argument to the command line utilities or by calling the `X509_VERIFY_PARAM_set1_policies()' function.</t>
+          <t>The NEX-Forms WordPress plugin before 8.3.3 does not have CSRF checks in place when editing a form, and does not escape some of its settings as well as form fields before outputting them in attributes. This could allow attackers to make a logged in admin edit arbitrary forms with Cross-Site Scripting payloads in them</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>2023-03-22T18:10:33.697</t>
+          <t>2023-03-17T09:15:10.680</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>CVE-2021-24705</t>
+          <t>CVE-2022-3837</t>
         </is>
       </c>
       <c r="B94" t="n">
@@ -2300,19 +2300,19 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>The NEX-Forms WordPress plugin before 8.3.3 does not have CSRF checks in place when editing a form, and does not escape some of its settings as well as form fields before outputting them in attributes. This could allow attackers to make a logged in admin edit arbitrary forms with Cross-Site Scripting payloads in them</t>
+          <t>The Uji Countdown WordPress plugin before 2.3.1 does not sanitise and escape some of its settings, which could allow high privilege users such as admin to perform Stored Cross-Site Scripting attacks even when the unfiltered_html capability is disallowed (for example in multisite setup).</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>2023-03-17T09:15:10.680</t>
+          <t>2023-03-17T09:15:11.833</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>CVE-2022-3837</t>
+          <t>CVE-2023-28155</t>
         </is>
       </c>
       <c r="B95" t="n">
@@ -2320,79 +2320,75 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>The Uji Countdown WordPress plugin before 2.3.1 does not sanitise and escape some of its settings, which could allow high privilege users such as admin to perform Stored Cross-Site Scripting attacks even when the unfiltered_html capability is disallowed (for example in multisite setup).</t>
+          <t>** UNSUPPORTED WHEN ASSIGNED ** The Request package through 2.88.1 for Node.js allows a bypass of SSRF mitigations via an attacker-controller server that does a cross-protocol redirect (HTTP to HTTPS, or HTTPS to HTTP). NOTE: This vulnerability only affects products that are no longer supported by the maintainer.</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>2023-03-17T09:15:11.833</t>
+          <t>2023-03-22T19:32:40.640</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>CVE-2023-23918</t>
+          <t>CVE-2021-46875</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>3.6</v>
+        <v>2.7</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>A privilege escalation vulnerability exists in Node.js &lt;19.6.1, &lt;18.14.1, &lt;16.19.1 and &lt;14.21.3 that made it possible to bypass the experimental Permissions (https://nodejs.org/api/permissions.html) feature in Node.js and access non authorized modules by using process.mainModule.require(). This only affects users who had enabled the experimental permissions option with --experimental-policy.</t>
+          <t>An issue was discovered in eZ Platform Ibexa Kernel before 1.3.1.1. An XSS attack can occur because JavaScript code can be uploaded in a .html or .js file.</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>2023-03-16T16:15:11.720</t>
+          <t>2023-03-16T18:21:25.523</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>CVE-2023-23920</t>
-        </is>
-      </c>
-      <c r="B97" t="n">
-        <v>3.6</v>
-      </c>
+          <t>CVE-2022-42333</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr"/>
       <c r="C97" t="inlineStr">
         <is>
-          <t>An untrusted search path vulnerability exists in Node.js. &lt;19.6.1, &lt;18.14.1, &lt;16.19.1, and &lt;14.21.3 that could allow an attacker to search and potentially load ICU data when running with elevated privileges.</t>
+          <t>x86/HVM pinned cache attributes mis-handling T[his CNA information record relates to multiple CVEs; the text explains which aspects/vulnerabilities correspond to which CVE.] To allow cachability control for HVM guests with passed through devices, an interface exists to explicitly override defaults which would otherwise be put in place. While not exposed to the affected guests themselves, the interface specifically exists for domains controlling such guests. This interface may therefore be used by not fully privileged entities, e.g. qemu running deprivileged in Dom0 or qemu running in a so called stub-domain. With this exposure it is an issue that - the number of the such controlled regions was unbounded (CVE-2022-42333), - installation and removal of such regions was not properly serialized (CVE-2022-42334).</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>2023-03-16T16:15:11.900</t>
+          <t>2023-03-21T15:15:12.040</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>CVE-2023-28155</t>
-        </is>
-      </c>
-      <c r="B98" t="n">
-        <v>2.7</v>
-      </c>
+          <t>CVE-2022-42334</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr"/>
       <c r="C98" t="inlineStr">
         <is>
-          <t>** UNSUPPORTED WHEN ASSIGNED ** The Request package through 2.88.1 for Node.js allows a bypass of SSRF mitigations via an attacker-controller server that does a cross-protocol redirect (HTTP to HTTPS, or HTTPS to HTTP). NOTE: This vulnerability only affects products that are no longer supported by the maintainer.</t>
+          <t>x86/HVM pinned cache attributes mis-handling T[his CNA information record relates to multiple CVEs; the text explains which aspects/vulnerabilities correspond to which CVE.] To allow cachability control for HVM guests with passed through devices, an interface exists to explicitly override defaults which would otherwise be put in place. While not exposed to the affected guests themselves, the interface specifically exists for domains controlling such guests. This interface may therefore be used by not fully privileged entities, e.g. qemu running deprivileged in Dom0 or qemu running in a so called stub-domain. With this exposure it is an issue that - the number of the such controlled regions was unbounded (CVE-2022-42333), - installation and removal of such regions was not properly serialized (CVE-2022-42334).</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>2023-03-22T19:32:40.640</t>
+          <t>2023-03-21T15:15:12.093</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>CVE-2021-46875</t>
+          <t>CVE-2023-26912</t>
         </is>
       </c>
       <c r="B99" t="n">
@@ -2400,151 +2396,155 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>An issue was discovered in eZ Platform Ibexa Kernel before 1.3.1.1. An XSS attack can occur because JavaScript code can be uploaded in a .html or .js file.</t>
+          <t>Cross site scripting (XSS) vulnerability in xenv S-mall-ssm thru commit 3d9e77f7d80289a30f67aaba1ae73e375d33ef71 on Feb 17, 2020, allows local attackers to execute arbitrary code via the evaluate button.</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>2023-03-16T18:21:25.523</t>
+          <t>2023-03-18T03:51:26.247</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>CVE-2022-42333</t>
+          <t>CVE-2022-42331</t>
         </is>
       </c>
       <c r="B100" t="inlineStr"/>
       <c r="C100" t="inlineStr">
         <is>
-          <t>x86/HVM pinned cache attributes mis-handling T[his CNA information record relates to multiple CVEs; the text explains which aspects/vulnerabilities correspond to which CVE.] To allow cachability control for HVM guests with passed through devices, an interface exists to explicitly override defaults which would otherwise be put in place. While not exposed to the affected guests themselves, the interface specifically exists for domains controlling such guests. This interface may therefore be used by not fully privileged entities, e.g. qemu running deprivileged in Dom0 or qemu running in a so called stub-domain. With this exposure it is an issue that - the number of the such controlled regions was unbounded (CVE-2022-42333), - installation and removal of such regions was not properly serialized (CVE-2022-42334).</t>
+          <t>x86: speculative vulnerability in 32bit SYSCALL path Due to an oversight in the very original Spectre/Meltdown security work (XSA-254), one entrypath performs its speculation-safety actions too late. In some configurations, there is an unprotected RET instruction which can be attacked with a variety of speculative attacks.</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>2023-03-21T15:15:12.040</t>
+          <t>2023-03-21T15:15:11.640</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>CVE-2022-42334</t>
+          <t>CVE-2022-42332</t>
         </is>
       </c>
       <c r="B101" t="inlineStr"/>
       <c r="C101" t="inlineStr">
         <is>
-          <t>x86/HVM pinned cache attributes mis-handling T[his CNA information record relates to multiple CVEs; the text explains which aspects/vulnerabilities correspond to which CVE.] To allow cachability control for HVM guests with passed through devices, an interface exists to explicitly override defaults which would otherwise be put in place. While not exposed to the affected guests themselves, the interface specifically exists for domains controlling such guests. This interface may therefore be used by not fully privileged entities, e.g. qemu running deprivileged in Dom0 or qemu running in a so called stub-domain. With this exposure it is an issue that - the number of the such controlled regions was unbounded (CVE-2022-42333), - installation and removal of such regions was not properly serialized (CVE-2022-42334).</t>
+          <t>x86 shadow plus log-dirty mode use-after-free In environments where host assisted address translation is necessary but Hardware Assisted Paging (HAP) is unavailable, Xen will run guests in so called shadow mode. Shadow mode maintains a pool of memory used for both shadow page tables as well as auxiliary data structures. To migrate or snapshot guests, Xen additionally runs them in so called log-dirty mode. The data structures needed by the log-dirty tracking are part of aformentioned auxiliary data. In order to keep error handling efforts within reasonable bounds, for operations which may require memory allocations shadow mode logic ensures up front that enough memory is available for the worst case requirements. Unfortunately, while page table memory is properly accounted for on the code path requiring the potential establishing of new shadows, demands by the log-dirty infrastructure were not taken into consideration. As a result, just established shadow page tables could be freed again immediately, while other code is still accessing them on the assumption that they would remain allocated.</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>2023-03-21T15:15:12.093</t>
+          <t>2023-03-21T15:15:11.847</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>CVE-2023-26912</t>
+          <t>CVE-2023-28425</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>2.7</v>
+        <v>3.6</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Cross site scripting (XSS) vulnerability in xenv S-mall-ssm thru commit 3d9e77f7d80289a30f67aaba1ae73e375d33ef71 on Feb 17, 2020, allows local attackers to execute arbitrary code via the evaluate button.</t>
+          <t>Redis is an in-memory database that persists on disk. Starting in version 7.0.8 and prior to version 7.0.10, authenticated users can use the MSETNX command to trigger a runtime assertion and termination of the Redis server process. The problem is fixed in Redis version 7.0.10.</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>2023-03-18T03:51:26.247</t>
+          <t>2023-03-21T11:51:09.643</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>CVE-2022-42331</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr"/>
+          <t>CVE-2023-27851</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>5.9</v>
+      </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>x86: speculative vulnerability in 32bit SYSCALL path Due to an oversight in the very original Spectre/Meltdown security work (XSA-254), one entrypath performs its speculation-safety actions too late. In some configurations, there is an unprotected RET instruction which can be attacked with a variety of speculative attacks.</t>
+          <t>NETGEAR Nighthawk WiFi6 Router prior to V1.0.10.94 contains a file sharing mechanism that unintentionally allows users with upload permissions to execute arbitrary code on the device.</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>2023-03-21T15:15:11.640</t>
+          <t>2023-03-16T17:18:10.443</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>CVE-2022-42332</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr"/>
+          <t>CVE-2023-1327</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>5.9</v>
+      </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>x86 shadow plus log-dirty mode use-after-free In environments where host assisted address translation is necessary but Hardware Assisted Paging (HAP) is unavailable, Xen will run guests in so called shadow mode. Shadow mode maintains a pool of memory used for both shadow page tables as well as auxiliary data structures. To migrate or snapshot guests, Xen additionally runs them in so called log-dirty mode. The data structures needed by the log-dirty tracking are part of aformentioned auxiliary data. In order to keep error handling efforts within reasonable bounds, for operations which may require memory allocations shadow mode logic ensures up front that enough memory is available for the worst case requirements. Unfortunately, while page table memory is properly accounted for on the code path requiring the potential establishing of new shadows, demands by the log-dirty infrastructure were not taken into consideration. As a result, just established shadow page tables could be freed again immediately, while other code is still accessing them on the assumption that they would remain allocated.</t>
+          <t>Netgear RAX30 (AX2400), prior to version 1.0.6.74, was affected by an authentication bypass vulnerability, allowing an unauthenticated attacker to gain administrative access to the device's web management interface by resetting the admin password.</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>2023-03-21T15:15:11.847</t>
+          <t>2023-03-21T17:59:23.193</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>CVE-2023-28425</t>
+          <t>CVE-2023-28337</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>3.6</v>
+        <v>5.9</v>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Redis is an in-memory database that persists on disk. Starting in version 7.0.8 and prior to version 7.0.10, authenticated users can use the MSETNX command to trigger a runtime assertion and termination of the Redis server process. The problem is fixed in Redis version 7.0.10.</t>
+          <t>When uploading a firmware image to a Netgear Nighthawk Wifi6 Router (RAX30), a hidden “forceFWUpdate” parameter may be provided to force the upgrade to complete and bypass certain validation checks. End users can use this to upload modified, unofficial, and potentially malicious firmware to the device.</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>2023-03-21T11:51:09.643</t>
+          <t>2023-03-21T17:40:15.477</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>CVE-2023-27851</t>
+          <t>CVE-2023-28338</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>5.9</v>
+        <v>3.6</v>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>NETGEAR Nighthawk WiFi6 Router prior to V1.0.10.94 contains a file sharing mechanism that unintentionally allows users with upload permissions to execute arbitrary code on the device.</t>
+          <t>Any request send to a Netgear Nighthawk Wifi6 Router (RAX30)'s web service containing a “Content-Type” of “multipartboundary=” will result in the request body being written to “/tmp/mulipartFile” on the device itself. A sufficiently large file will cause device resources to be exhausted, resulting in the device becoming unusable until it is rebooted.</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>2023-03-16T17:18:10.443</t>
+          <t>2023-03-21T17:57:33.130</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>CVE-2023-1327</t>
+          <t>CVE-2022-36429</t>
         </is>
       </c>
       <c r="B107" t="n">
@@ -2552,19 +2552,19 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Netgear RAX30 (AX2400), prior to version 1.0.6.74, was affected by an authentication bypass vulnerability, allowing an unauthenticated attacker to gain administrative access to the device's web management interface by resetting the admin password.</t>
+          <t>A command execution vulnerability exists in the ubus backend communications functionality of Netgear Orbi Satellite RBS750 4.6.8.5. A specially-crafted JSON object can lead to arbitrary command execution. An attacker can send a sequence of malicious packets to trigger this vulnerability.</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>2023-03-21T17:59:23.193</t>
+          <t>2023-03-21T20:07:21.987</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>CVE-2023-28337</t>
+          <t>CVE-2023-24762</t>
         </is>
       </c>
       <c r="B108" t="n">
@@ -2572,59 +2572,59 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>When uploading a firmware image to a Netgear Nighthawk Wifi6 Router (RAX30), a hidden “forceFWUpdate” parameter may be provided to force the upgrade to complete and bypass certain validation checks. End users can use this to upload modified, unofficial, and potentially malicious firmware to the device.</t>
+          <t>OS Command injection vulnerability in D-Link DIR-867 DIR_867_FW1.30B07 allows attackers to execute arbitrary commands via a crafted LocalIPAddress parameter for the SetVirtualServerSettings to HNAP1.</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>2023-03-21T17:40:15.477</t>
+          <t>2023-03-17T04:02:59.983</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>CVE-2023-28338</t>
+          <t>CVE-2023-25279</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>3.6</v>
+        <v>5.9</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Any request send to a Netgear Nighthawk Wifi6 Router (RAX30)'s web service containing a “Content-Type” of “multipartboundary=” will result in the request body being written to “/tmp/mulipartFile” on the device itself. A sufficiently large file will cause device resources to be exhausted, resulting in the device becoming unusable until it is rebooted.</t>
+          <t>OS Command injection vulnerability in D-Link DIR820LA1_FW105B03 allows attackers to escalate privileges to root via a crafted payload.</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>2023-03-21T17:57:33.130</t>
+          <t>2023-03-17T03:51:01.730</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>CVE-2022-36429</t>
+          <t>CVE-2023-25282</t>
         </is>
       </c>
       <c r="B110" t="n">
-        <v>5.9</v>
+        <v>3.6</v>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>A command execution vulnerability exists in the ubus backend communications functionality of Netgear Orbi Satellite RBS750 4.6.8.5. A specially-crafted JSON object can lead to arbitrary command execution. An attacker can send a sequence of malicious packets to trigger this vulnerability.</t>
+          <t>A heap overflow vulnerability in D-Link DIR820LA1_FW106B02 allows attackers to cause a denial of service via the config.log_to_syslog and log_opt_dropPackets parameters to mydlink_api.ccp.</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>2023-03-21T20:07:21.987</t>
+          <t>2023-03-18T03:58:08.180</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>CVE-2023-24762</t>
+          <t>CVE-2023-25280</t>
         </is>
       </c>
       <c r="B111" t="n">
@@ -2632,391 +2632,389 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>OS Command injection vulnerability in D-Link DIR-867 DIR_867_FW1.30B07 allows attackers to execute arbitrary commands via a crafted LocalIPAddress parameter for the SetVirtualServerSettings to HNAP1.</t>
+          <t>OS Command injection vulnerability in D-Link DIR820LA1_FW105B03 allows attackers to escalate privileges to root via a crafted payload with the ping_addr parameter to ping.ccp.</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>2023-03-17T04:02:59.983</t>
+          <t>2023-03-21T17:33:33.767</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>CVE-2023-25279</t>
+          <t>CVE-2023-1410</t>
         </is>
       </c>
       <c r="B112" t="n">
-        <v>5.9</v>
+        <v>4.7</v>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>OS Command injection vulnerability in D-Link DIR820LA1_FW105B03 allows attackers to escalate privileges to root via a crafted payload.</t>
+          <t>Grafana is an open-source platform for monitoring and observability. Grafana had a stored XSS vulnerability in the Graphite FunctionDescription tooltip. The stored XSS vulnerability was possible due the value of the Function Description was not properly sanitized. An attacker needs to have control over the Graphite data source in order to manipulate a function description and a Grafana admin needs to configure the data source, later a Grafana user needs to select a tampered function and hover over the description. Users may upgrade to version 8.5.22, 9.2.15 and 9.3.11 to receive a fix.</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>2023-03-17T03:51:01.730</t>
+          <t>2023-03-23T13:41:53.480</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>CVE-2023-25282</t>
+          <t>CVE-2023-1358</t>
         </is>
       </c>
       <c r="B113" t="n">
-        <v>3.6</v>
+        <v>5.9</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>A heap overflow vulnerability in D-Link DIR820LA1_FW106B02 allows attackers to cause a denial of service via the config.log_to_syslog and log_opt_dropPackets parameters to mydlink_api.ccp.</t>
+          <t>A vulnerability, which was classified as critical, was found in SourceCodester Gadget Works Online Ordering System 1.0. This affects an unknown part of the file /philosophy/admin/login.php of the component POST Parameter Handler. The manipulation of the argument user_email leads to sql injection. It is possible to initiate the attack remotely. The exploit has been disclosed to the public and may be used. The identifier VDB-222861 was assigned to this vulnerability.</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>2023-03-18T03:58:08.180</t>
+          <t>2023-03-17T03:56:20.807</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>CVE-2023-25280</t>
+          <t>CVE-2023-1359</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>5.9</v>
+        <v>2.7</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>OS Command injection vulnerability in D-Link DIR820LA1_FW105B03 allows attackers to escalate privileges to root via a crafted payload with the ping_addr parameter to ping.ccp.</t>
+          <t>A vulnerability has been found in SourceCodester Gadget Works Online Ordering System 1.0 and classified as problematic. This vulnerability affects unknown code of the file /philosophy/admin/user/controller.php?action=add of the component Add New User. The manipulation of the argument U_NAME leads to cross site scripting. The attack can be initiated remotely. The exploit has been disclosed to the public and may be used. VDB-222862 is the identifier assigned to this vulnerability.</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>2023-03-21T17:33:33.767</t>
+          <t>2023-03-17T03:56:04.487</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>CVE-2023-1410</t>
+          <t>CVE-2023-1364</t>
         </is>
       </c>
       <c r="B115" t="n">
-        <v>4.7</v>
+        <v>3.6</v>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Grafana is an open-source platform for monitoring and observability. Grafana had a stored XSS vulnerability in the Graphite FunctionDescription tooltip. The stored XSS vulnerability was possible due the value of the Function Description was not properly sanitized. An attacker needs to have control over the Graphite data source in order to manipulate a function description and a Grafana admin needs to configure the data source, later a Grafana user needs to select a tampered function and hover over the description. Users may upgrade to version 8.5.22, 9.2.15 and 9.3.11 to receive a fix.</t>
+          <t>A vulnerability has been found in SourceCodester Online Pizza Ordering System 1.0 and classified as critical. Affected by this vulnerability is an unknown functionality of the file category.php of the component GET Parameter Handler. The manipulation of the argument id leads to sql injection. The attack can be launched remotely. The exploit has been disclosed to the public and may be used. The associated identifier of this vulnerability is VDB-222871.</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>2023-03-23T13:41:53.480</t>
+          <t>2023-03-17T03:55:16.137</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>CVE-2023-28100</t>
+          <t>CVE-2012-3024</t>
         </is>
       </c>
       <c r="B116" t="n">
-        <v>6</v>
+        <v>2.9</v>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Flatpak is a system for building, distributing, and running sandboxed desktop applications on Linux. Versions prior to 1.10.8, 1.12.8, 1.14.4, and 1.15.4 contain a vulnerability similar to CVE-2017-5226, but using the `TIOCLINUX` ioctl command instead of `TIOCSTI`. If a Flatpak app is run on a Linux virtual console such as `/dev/tty1`, it can copy text from the virtual console and paste it into the command buffer, from which the command might be run after the Flatpak app has exited. Ordinary graphical terminal emulators like xterm, gnome-terminal and Konsole are unaffected. This vulnerability is specific to the Linux virtual consoles `/dev/tty1`, `/dev/tty2` and so on. A patch is available in versions 1.10.8, 1.12.8, 1.14.4, and 1.15.4. As a workaround, don't run Flatpak on a Linux virtual console. Flatpak is primarily designed to be used in a Wayland or X11 graphical environment.</t>
+          <t>Tridium Niagara AX Framework through 3.6 uses predictable values for (1) session IDs and (2) keys, which might allow remote attackers to bypass authentication via a brute-force attack.</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>2023-03-22T19:13:43.267</t>
+          <t>2023-03-22T14:08:50.977</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>CVE-2023-1358</t>
+          <t>CVE-2012-3025</t>
         </is>
       </c>
       <c r="B117" t="n">
-        <v>5.9</v>
+        <v>2.9</v>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>A vulnerability, which was classified as critical, was found in SourceCodester Gadget Works Online Ordering System 1.0. This affects an unknown part of the file /philosophy/admin/login.php of the component POST Parameter Handler. The manipulation of the argument user_email leads to sql injection. It is possible to initiate the attack remotely. The exploit has been disclosed to the public and may be used. The identifier VDB-222861 was assigned to this vulnerability.</t>
+          <t>The default configuration of Tridium Niagara AX Framework through 3.6 uses a cleartext base64 format for transmission of credentials in cookies, which allows remote attackers to obtain sensitive information by sniffing the network.</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>2023-03-17T03:56:20.807</t>
+          <t>2023-03-22T14:09:30.673</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>CVE-2023-1359</t>
+          <t>CVE-2012-4701</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>2.7</v>
+        <v>10</v>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>A vulnerability has been found in SourceCodester Gadget Works Online Ordering System 1.0 and classified as problematic. This vulnerability affects unknown code of the file /philosophy/admin/user/controller.php?action=add of the component Add New User. The manipulation of the argument U_NAME leads to cross site scripting. The attack can be initiated remotely. The exploit has been disclosed to the public and may be used. VDB-222862 is the identifier assigned to this vulnerability.</t>
+          <t>Directory traversal vulnerability in Tridium Niagara AX 3.5, 3.6, and 3.7 allows remote attackers to read sensitive files, and consequently execute arbitrary code, by leveraging (1) valid credentials or (2) the guest feature.</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>2023-03-17T03:56:04.487</t>
+          <t>2023-03-22T14:11:31.713</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>CVE-2012-3024</t>
+          <t>CVE-2023-27239</t>
         </is>
       </c>
       <c r="B119" t="n">
-        <v>2.9</v>
+        <v>5.9</v>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Tridium Niagara AX Framework through 3.6 uses predictable values for (1) session IDs and (2) keys, which might allow remote attackers to bypass authentication via a brute-force attack.</t>
+          <t>Tenda AX3 V16.03.12.11 was discovered to contain a stack overflow via the shareSpeed parameter at /goform/WifiGuestSet.</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>2023-03-22T14:08:50.977</t>
+          <t>2023-03-21T15:04:58.160</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>CVE-2012-3025</t>
+          <t>CVE-2023-27240</t>
         </is>
       </c>
       <c r="B120" t="n">
-        <v>2.9</v>
+        <v>5.9</v>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>The default configuration of Tridium Niagara AX Framework through 3.6 uses a cleartext base64 format for transmission of credentials in cookies, which allows remote attackers to obtain sensitive information by sniffing the network.</t>
+          <t>Tenda AX3 V16.03.12.11 was discovered to contain a command injection vulnerability via the lanip parameter at /goform/AdvSetLanip.</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>2023-03-22T14:09:30.673</t>
+          <t>2023-03-21T15:04:28.480</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>CVE-2012-4701</t>
-        </is>
-      </c>
-      <c r="B121" t="n">
-        <v>10</v>
-      </c>
+          <t>CVE-2023-26805</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr"/>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Directory traversal vulnerability in Tridium Niagara AX 3.5, 3.6, and 3.7 allows remote attackers to read sensitive files, and consequently execute arbitrary code, by leveraging (1) valid credentials or (2) the guest feature.</t>
+          <t>Tenda W20E v15.11.0.6 (US_W20EV4.0br_v15.11.0.6(1068_1546_841)_CN_TDC) is vulnerable to Buffer Overflow via function formIPMacBindModify.</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>2023-03-22T14:11:31.713</t>
+          <t>2023-03-20T02:46:58.537</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>CVE-2023-27239</t>
-        </is>
-      </c>
-      <c r="B122" t="n">
-        <v>5.9</v>
-      </c>
+          <t>CVE-2023-26806</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr"/>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Tenda AX3 V16.03.12.11 was discovered to contain a stack overflow via the shareSpeed parameter at /goform/WifiGuestSet.</t>
+          <t>Tenda W20E v15.11.0.6(US_W20EV4.0br_v15.11.0.6(1068_1546_841 is vulnerable to Buffer Overflow via function formSetSysTime,</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>2023-03-21T15:04:58.160</t>
+          <t>2023-03-20T02:46:58.537</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>CVE-2023-27240</t>
-        </is>
-      </c>
-      <c r="B123" t="n">
-        <v>5.9</v>
-      </c>
+          <t>CVE-2023-27079</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr"/>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Tenda AX3 V16.03.12.11 was discovered to contain a command injection vulnerability via the lanip parameter at /goform/AdvSetLanip.</t>
+          <t>Command Injection vulnerability found in Tenda G103 v.1.0.05 allows an attacker to obtain sensitive information via a crafted package</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>2023-03-21T15:04:28.480</t>
+          <t>2023-03-23T14:42:05.620</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>CVE-2023-26805</t>
+          <t>CVE-2023-1306</t>
         </is>
       </c>
       <c r="B124" t="inlineStr"/>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Tenda W20E v15.11.0.6 (US_W20EV4.0br_v15.11.0.6(1068_1546_841)_CN_TDC) is vulnerable to Buffer Overflow via function formIPMacBindModify.</t>
+          <t>An authenticated attacker can leverage an exposed resource.db() accessor method to smuggle Python method calls via a Jinja template, which can lead to code execution. This issue was resolved in the Managed and SaaS deployments on February 1, 2023, and in version 23.2.1 of the Self-Managed version of InsightCloudSec.</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>2023-03-20T02:46:58.537</t>
+          <t>2023-03-21T20:07:21.987</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>CVE-2023-26806</t>
-        </is>
-      </c>
-      <c r="B125" t="inlineStr"/>
+          <t>CVE-2018-25082</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
+        <v>3.4</v>
+      </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Tenda W20E v15.11.0.6(US_W20EV4.0br_v15.11.0.6(1068_1546_841 is vulnerable to Buffer Overflow via function formSetSysTime,</t>
+          <t>A vulnerability was found in zwczou WeChat SDK Python 0.3.0 and classified as critical. This issue affects the function validate/to_xml. The manipulation leads to xml external entity reference. The attack may be initiated remotely. Upgrading to version 0.5.5 is able to address this issue. The name of the patch is e54abadc777715b6dcb545c13214d1dea63df6c9. It is recommended to upgrade the affected component. The associated identifier of this vulnerability is VDB-223403.</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>2023-03-20T02:46:58.537</t>
+          <t>2023-03-21T20:07:21.987</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>CVE-2023-27079</t>
-        </is>
-      </c>
-      <c r="B126" t="inlineStr"/>
+          <t>CVE-2023-28117</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>4.7</v>
+      </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Command Injection vulnerability found in Tenda G103 v.1.0.05 allows an attacker to obtain sensitive information via a crafted package</t>
+          <t>Sentry SDK is the official Python SDK for Sentry, real-time crash reporting software. When using the Django integration of versions prior to 1.14.0 of the Sentry SDK in a specific configuration it is possible to leak sensitive cookies values, including the session cookie to Sentry. These sensitive cookies could then be used by someone with access to your Sentry issues to impersonate or escalate their privileges within your application. In order for these sensitive values to be leaked, the Sentry SDK configuration must have `sendDefaultPII` set to `True`; one must use a custom name for either `SESSION_COOKIE_NAME` or `CSRF_COOKIE_NAME` in one's Django settings; and one must not be configured in one's organization or project settings to use Sentry's data scrubbing features to account for the custom cookie names. As of version 1.14.0, the Django integration of the `sentry-sdk` will detect the custom cookie names based on one's Django settings and will remove the values from the payload before sending the data to Sentry. As a workaround, use the SDK's filtering mechanism to remove the cookies from the payload that is sent to Sentry. For error events, this can be done with the `before_send` callback method and for performance related events (transactions) one can use the `before_send_transaction` callback method. Those who want to handle filtering of these values on the server-side can also use Sentry's advanced data scrubbing feature to account for the custom cookie names. Look for the `$http.cookies`, `$http.headers`, `$request.cookies`, or `$request.headers` fields to target with a scrubbing rule.</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>2023-03-23T14:42:05.620</t>
+          <t>2023-03-23T01:03:10.803</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>CVE-2023-1306</t>
-        </is>
-      </c>
-      <c r="B127" t="inlineStr"/>
+          <t>CVE-2023-28431</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>3.6</v>
+      </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>An authenticated attacker can leverage an exposed resource.db() accessor method to smuggle Python method calls via a Jinja template, which can lead to code execution. This issue was resolved in the Managed and SaaS deployments on February 1, 2023, and in version 23.2.1 of the Self-Managed version of InsightCloudSec.</t>
+          <t>Frontier is an Ethereum compatibility layer for Substrate. Frontier's `modexp` precompile uses `num-bigint` crate under the hood. In the implementation prior to pull request 1017, the cases for modulus being even and modulus being odd are treated separately. Odd modulus uses the fast Montgomery multiplication, and even modulus uses the slow plain power algorithm. This gas cost discrepancy was not accounted for in the `modexp` precompile, leading to possible denial of service attacks. No fixes for `num-bigint` are currently available, and thus this issue is fixed in the short term by raising the gas costs for even modulus, and in the long term fixing it in `num-bigint` or switching to another modexp implementation. The short-term fix for Frontier is deployed at pull request 1017. There are no known workarounds aside from applying the fix.</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>2023-03-21T20:07:21.987</t>
+          <t>2023-03-23T01:02:56.037</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>CVE-2018-25082</t>
+          <t>CVE-2023-27902</t>
         </is>
       </c>
       <c r="B128" t="n">
-        <v>3.4</v>
+        <v>1.4</v>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>A vulnerability was found in zwczou WeChat SDK Python 0.3.0 and classified as critical. This issue affects the function validate/to_xml. The manipulation leads to xml external entity reference. The attack may be initiated remotely. Upgrading to version 0.5.5 is able to address this issue. The name of the patch is e54abadc777715b6dcb545c13214d1dea63df6c9. It is recommended to upgrade the affected component. The associated identifier of this vulnerability is VDB-223403.</t>
+          <t>Jenkins 2.393 and earlier, LTS 2.375.3 and earlier shows temporary directories related to job workspaces, which allows attackers with Item/Workspace permission to access their contents.</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>2023-03-21T20:07:21.987</t>
+          <t>2023-03-16T17:15:39.150</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>CVE-2023-28117</t>
-        </is>
-      </c>
-      <c r="B129" t="n">
-        <v>4.7</v>
-      </c>
+          <t>CVE-2023-28685</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr"/>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Sentry SDK is the official Python SDK for Sentry, real-time crash reporting software. When using the Django integration of versions prior to 1.14.0 of the Sentry SDK in a specific configuration it is possible to leak sensitive cookies values, including the session cookie to Sentry. These sensitive cookies could then be used by someone with access to your Sentry issues to impersonate or escalate their privileges within your application. In order for these sensitive values to be leaked, the Sentry SDK configuration must have `sendDefaultPII` set to `True`; one must use a custom name for either `SESSION_COOKIE_NAME` or `CSRF_COOKIE_NAME` in one's Django settings; and one must not be configured in one's organization or project settings to use Sentry's data scrubbing features to account for the custom cookie names. As of version 1.14.0, the Django integration of the `sentry-sdk` will detect the custom cookie names based on one's Django settings and will remove the values from the payload before sending the data to Sentry. As a workaround, use the SDK's filtering mechanism to remove the cookies from the payload that is sent to Sentry. For error events, this can be done with the `before_send` callback method and for performance related events (transactions) one can use the `before_send_transaction` callback method. Those who want to handle filtering of these values on the server-side can also use Sentry's advanced data scrubbing feature to account for the custom cookie names. Look for the `$http.cookies`, `$http.headers`, `$request.cookies`, or `$request.headers` fields to target with a scrubbing rule.</t>
+          <t>Jenkins AbsInt a³ Plugin 1.1.0 and earlier does not configure its XML parser to prevent XML external entity (XXE) attacks.</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>2023-03-23T01:03:10.803</t>
+          <t>2023-03-22T12:47:56.330</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>CVE-2023-28431</t>
+          <t>CVE-2023-24999</t>
         </is>
       </c>
       <c r="B130" t="n">
-        <v>3.6</v>
+        <v>5.2</v>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Frontier is an Ethereum compatibility layer for Substrate. Frontier's `modexp` precompile uses `num-bigint` crate under the hood. In the implementation prior to pull request 1017, the cases for modulus being even and modulus being odd are treated separately. Odd modulus uses the fast Montgomery multiplication, and even modulus uses the slow plain power algorithm. This gas cost discrepancy was not accounted for in the `modexp` precompile, leading to possible denial of service attacks. No fixes for `num-bigint` are currently available, and thus this issue is fixed in the short term by raising the gas costs for even modulus, and in the long term fixing it in `num-bigint` or switching to another modexp implementation. The short-term fix for Frontier is deployed at pull request 1017. There are no known workarounds aside from applying the fix.</t>
+          <t>HashiCorp Vault and Vault Enterprise’s approle auth method allowed any authenticated user with access to an approle destroy endpoint to destroy the secret ID of any other role by providing the secret ID accessor. This vulnerability is fixed in Vault 1.13.0, 1.12.4, 1.11.8, 1.10.11 and above.</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>2023-03-23T01:02:56.037</t>
+          <t>2023-03-16T17:03:07.880</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>CVE-2023-27902</t>
+          <t>CVE-2023-1296</t>
         </is>
       </c>
       <c r="B131" t="n">
@@ -3024,77 +3022,79 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Jenkins 2.393 and earlier, LTS 2.375.3 and earlier shows temporary directories related to job workspaces, which allows attackers with Item/Workspace permission to access their contents.</t>
+          <t>HashiCorp Nomad and Nomad Enterprise 1.4.0 up to 1.5.0 did not correctly enforce deny policies applied to a workload’s variables. Fixed in 1.4.6 and 1.5.1.</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>2023-03-16T17:15:39.150</t>
+          <t>2023-03-17T03:58:51.637</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>CVE-2023-28685</t>
-        </is>
-      </c>
-      <c r="B132" t="inlineStr"/>
+          <t>CVE-2023-1299</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
+        <v>5.9</v>
+      </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Jenkins AbsInt a³ Plugin 1.1.0 and earlier does not configure its XML parser to prevent XML external entity (XXE) attacks.</t>
+          <t>HashiCorp Nomad and Nomad Enterprise 1.5.0 allow a job submitter to escalate to management-level privileges using workload identity and task API. Fixed in 1.5.1.</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>2023-03-22T12:47:56.330</t>
+          <t>2023-03-17T03:58:33.453</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>CVE-2023-24999</t>
+          <t>CVE-2022-4933</t>
         </is>
       </c>
       <c r="B133" t="n">
-        <v>5.2</v>
+        <v>3.4</v>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>HashiCorp Vault and Vault Enterprise’s approle auth method allowed any authenticated user with access to an approle destroy endpoint to destroy the secret ID of any other role by providing the secret ID accessor. This vulnerability is fixed in Vault 1.13.0, 1.12.4, 1.11.8, 1.10.11 and above.</t>
+          <t>A vulnerability, which was classified as critical, has been found in ATM Consulting dolibarr_module_quicksupplierprice up to 1.1.6. Affected by this issue is the function upatePrice of the file script/interface.php. The manipulation leads to sql injection. The attack may be launched remotely. Upgrading to version 1.1.7 is able to address this issue. The name of the patch is ccad1e4282b0e393a32fcc852e82ec0e0af5446f. It is recommended to upgrade the affected component. VDB-223382 is the identifier assigned to this vulnerability.</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>2023-03-16T17:03:07.880</t>
+          <t>2023-03-20T14:02:42.383</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>CVE-2023-1296</t>
+          <t>CVE-2022-41418</t>
         </is>
       </c>
       <c r="B134" t="n">
-        <v>1.4</v>
+        <v>5.9</v>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>HashiCorp Nomad and Nomad Enterprise 1.4.0 up to 1.5.0 did not correctly enforce deny policies applied to a workload’s variables. Fixed in 1.4.6 and 1.5.1.</t>
+          <t>An issue in the component BlogEngine/BlogEngine.NET/AppCode/Api/UploadController.cs of BlogEngine.NET v3.3.8.0 allows attackers to execute arbitrary code via uploading a crafted PNG file.</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>2023-03-17T03:58:51.637</t>
+          <t>2023-03-22T00:15:12.163</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>CVE-2023-1299</t>
+          <t>CVE-2023-1366</t>
         </is>
       </c>
       <c r="B135" t="n">
@@ -3102,39 +3102,39 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>HashiCorp Nomad and Nomad Enterprise 1.5.0 allow a job submitter to escalate to management-level privileges using workload identity and task API. Fixed in 1.5.1.</t>
+          <t>A vulnerability was found in SourceCodester Yoga Class Registration System 1.0. It has been classified as critical. This affects the function query of the file admin/categories/manage_category.php. The manipulation of the argument id leads to sql injection. It is possible to initiate the attack remotely. The exploit has been disclosed to the public and may be used. The identifier VDB-222873 was assigned to this vulnerability.</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>2023-03-17T03:58:33.453</t>
+          <t>2023-03-17T03:54:15.037</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>CVE-2022-4933</t>
+          <t>CVE-2023-24577</t>
         </is>
       </c>
       <c r="B136" t="n">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>A vulnerability, which was classified as critical, has been found in ATM Consulting dolibarr_module_quicksupplierprice up to 1.1.6. Affected by this issue is the function upatePrice of the file script/interface.php. The manipulation leads to sql injection. The attack may be launched remotely. Upgrading to version 1.1.7 is able to address this issue. The name of the patch is ccad1e4282b0e393a32fcc852e82ec0e0af5446f. It is recommended to upgrade the affected component. VDB-223382 is the identifier assigned to this vulnerability.</t>
+          <t>McAfee Total Protection prior to 16.0.50 allows attackers to elevate user privileges due to Improper Link Resolution via registry keys. This could enable a user with lower privileges to execute unauthorized tasks.</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>2023-03-20T14:02:42.383</t>
+          <t>2023-03-22T19:37:04.393</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>CVE-2022-41418</t>
+          <t>CVE-2023-25991</t>
         </is>
       </c>
       <c r="B137" t="n">
@@ -3142,19 +3142,19 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>An issue in the component BlogEngine/BlogEngine.NET/AppCode/Api/UploadController.cs of BlogEngine.NET v3.3.8.0 allows attackers to execute arbitrary code via uploading a crafted PNG file.</t>
+          <t>Cross-Site Request Forgery (CSRF) vulnerability in RegistrationMagic plugin &lt;= 5.1.9.2 versions.</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>2023-03-22T00:15:12.163</t>
+          <t>2023-03-16T19:53:18.713</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>CVE-2023-1366</t>
+          <t>CVE-2023-27590</t>
         </is>
       </c>
       <c r="B138" t="n">
@@ -3162,59 +3162,59 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>A vulnerability was found in SourceCodester Yoga Class Registration System 1.0. It has been classified as critical. This affects the function query of the file admin/categories/manage_category.php. The manipulation of the argument id leads to sql injection. It is possible to initiate the attack remotely. The exploit has been disclosed to the public and may be used. The identifier VDB-222873 was assigned to this vulnerability.</t>
+          <t>Rizin is a UNIX-like reverse engineering framework and command-line toolset. In version 0.5.1 and prior, converting a GDB registers profile file into a Rizin register profile can result in a stack-based buffer overflow when the `name`, `type`, or `groups` fields have longer values than expected. Users opening untrusted GDB registers files (e.g. with the `drpg` or `arpg` commands) are affected by this flaw. Commit d6196703d89c84467b600ba2692534579dc25ed4 contains a patch for this issue. As a workaround, review the GDB register profiles before loading them with `drpg`/`arpg` commands.</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>2023-03-17T03:54:15.037</t>
+          <t>2023-03-21T15:00:44.043</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>CVE-2023-24577</t>
+          <t>CVE-2023-23389</t>
         </is>
       </c>
       <c r="B139" t="n">
-        <v>3.6</v>
+        <v>5.2</v>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>McAfee Total Protection prior to 16.0.50 allows attackers to elevate user privileges due to Improper Link Resolution via registry keys. This could enable a user with lower privileges to execute unauthorized tasks.</t>
+          <t>Microsoft Defender Elevation of Privilege Vulnerability</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>2023-03-22T19:37:04.393</t>
+          <t>2023-03-20T16:42:30.047</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>CVE-2023-25991</t>
+          <t>CVE-2023-23395</t>
         </is>
       </c>
       <c r="B140" t="n">
-        <v>5.9</v>
+        <v>1.4</v>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Cross-Site Request Forgery (CSRF) vulnerability in RegistrationMagic plugin &lt;= 5.1.9.2 versions.</t>
+          <t>Microsoft SharePoint Server Spoofing Vulnerability</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>2023-03-16T19:53:18.713</t>
+          <t>2023-03-20T21:19:19.997</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>CVE-2023-27590</t>
+          <t>CVE-2023-23397</t>
         </is>
       </c>
       <c r="B141" t="n">
@@ -3222,59 +3222,59 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Rizin is a UNIX-like reverse engineering framework and command-line toolset. In version 0.5.1 and prior, converting a GDB registers profile file into a Rizin register profile can result in a stack-based buffer overflow when the `name`, `type`, or `groups` fields have longer values than expected. Users opening untrusted GDB registers files (e.g. with the `drpg` or `arpg` commands) are affected by this flaw. Commit d6196703d89c84467b600ba2692534579dc25ed4 contains a patch for this issue. As a workaround, review the GDB register profiles before loading them with `drpg`/`arpg` commands.</t>
+          <t>Microsoft Outlook Elevation of Privilege Vulnerability</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>2023-03-21T15:00:44.043</t>
+          <t>2023-03-20T14:00:48.040</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>CVE-2023-23389</t>
+          <t>CVE-2023-23396</t>
         </is>
       </c>
       <c r="B142" t="n">
-        <v>5.2</v>
+        <v>3.6</v>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Microsoft Defender Elevation of Privilege Vulnerability</t>
+          <t>Microsoft Excel Denial of Service Vulnerability</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>2023-03-20T16:42:30.047</t>
+          <t>2023-03-20T21:20:32.613</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>CVE-2023-23395</t>
+          <t>CVE-2023-23398</t>
         </is>
       </c>
       <c r="B143" t="n">
-        <v>1.4</v>
+        <v>3.6</v>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Microsoft SharePoint Server Spoofing Vulnerability</t>
+          <t>Microsoft Excel Spoofing Vulnerability</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>2023-03-20T21:19:19.997</t>
+          <t>2023-03-20T21:22:32.353</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>CVE-2023-23397</t>
+          <t>CVE-2023-23399</t>
         </is>
       </c>
       <c r="B144" t="n">
@@ -3282,19 +3282,19 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Microsoft Outlook Elevation of Privilege Vulnerability</t>
+          <t>Microsoft Excel Remote Code Execution Vulnerability</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>2023-03-20T14:00:48.040</t>
+          <t>2023-03-20T21:22:44.917</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>CVE-2023-23396</t>
+          <t>CVE-2021-29446</t>
         </is>
       </c>
       <c r="B145" t="n">
@@ -3302,39 +3302,39 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>Microsoft Excel Denial of Service Vulnerability</t>
+          <t>jose-node-cjs-runtime is an npm package which provides a number of cryptographic functions. In versions prior to 3.11.4 the AES_CBC_HMAC_SHA2 Algorithm (A128CBC-HS256, A192CBC-HS384, A256CBC-HS512) decryption would always execute both HMAC tag verification and CBC decryption, if either failed `JWEDecryptionFailed` would be thrown. But a possibly observable difference in timing when padding error would occur while decrypting the ciphertext makes a padding oracle and an adversary might be able to make use of that oracle to decrypt data without knowing the decryption key by issuing on average 128*b calls to the padding oracle (where b is the number of bytes in the ciphertext block). A patch was released which ensures the HMAC tag is verified before performing CBC decryption. The fixed versions are `&gt;=3.11.4`. Users should upgrade to `^3.11.4`.</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>2023-03-20T21:20:32.613</t>
+          <t>2023-03-21T13:19:29.667</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>CVE-2023-23398</t>
+          <t>CVE-2023-27074</t>
         </is>
       </c>
       <c r="B146" t="n">
-        <v>3.6</v>
+        <v>5.9</v>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Microsoft Excel Spoofing Vulnerability</t>
+          <t>BP Monitoring Management System v1.0 was discovered to contain a SQL injection vulnerability via the emailid parameter in the login page.</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>2023-03-20T21:22:32.353</t>
+          <t>2023-03-17T03:57:52.503</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>CVE-2023-23399</t>
+          <t>CVE-2023-24726</t>
         </is>
       </c>
       <c r="B147" t="n">
@@ -3342,371 +3342,371 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Microsoft Excel Remote Code Execution Vulnerability</t>
+          <t>Art Gallery Management System v1.0 was discovered to contain a SQL injection vulnerability via the viewid parameter on the enquiry page.</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>2023-03-20T21:22:44.917</t>
+          <t>2023-03-17T18:19:15.197</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>CVE-2021-29446</t>
+          <t>CVE-2023-1421</t>
         </is>
       </c>
       <c r="B148" t="n">
-        <v>3.6</v>
+        <v>2.7</v>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>jose-node-cjs-runtime is an npm package which provides a number of cryptographic functions. In versions prior to 3.11.4 the AES_CBC_HMAC_SHA2 Algorithm (A128CBC-HS256, A192CBC-HS384, A256CBC-HS512) decryption would always execute both HMAC tag verification and CBC decryption, if either failed `JWEDecryptionFailed` would be thrown. But a possibly observable difference in timing when padding error would occur while decrypting the ciphertext makes a padding oracle and an adversary might be able to make use of that oracle to decrypt data without knowing the decryption key by issuing on average 128*b calls to the padding oracle (where b is the number of bytes in the ciphertext block). A patch was released which ensures the HMAC tag is verified before performing CBC decryption. The fixed versions are `&gt;=3.11.4`. Users should upgrade to `^3.11.4`.</t>
+          <t>A reflected cross-site scripting vulnerability in the OAuth flow completion endpoints in Mattermost allows an attacker to send AJAX requests on behalf of the victim via sharing a crafted link with a malicious state parameter.</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>2023-03-21T13:19:29.667</t>
+          <t>2023-03-21T15:26:57.867</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>CVE-2023-27074</t>
+          <t>CVE-2023-1562</t>
         </is>
       </c>
       <c r="B149" t="n">
-        <v>5.9</v>
+        <v>1.4</v>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>BP Monitoring Management System v1.0 was discovered to contain a SQL injection vulnerability via the emailid parameter in the login page.</t>
+          <t>Mattermost fails to check the "Show Full Name" setting when rendering the result for the /plugins/focalboard/api/v2/users API call, allowing an attacker to learn the full name of a board owner.</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>2023-03-17T03:57:52.503</t>
+          <t>2023-03-22T12:47:56.330</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>CVE-2023-24726</t>
+          <t>CVE-2023-22680</t>
         </is>
       </c>
       <c r="B150" t="n">
-        <v>5.9</v>
+        <v>2.7</v>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>Art Gallery Management System v1.0 was discovered to contain a SQL injection vulnerability via the viewid parameter on the enquiry page.</t>
+          <t>Auth. (admin+) Stored Cross-Site Scripting (XSS) vulnerability in Altanic No API Amazon Affiliate plugin &lt;= 4.2.2 versions.</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>2023-03-17T18:19:15.197</t>
+          <t>2023-03-23T15:07:27.350</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>CVE-2023-1421</t>
+          <t>CVE-2022-27782</t>
         </is>
       </c>
       <c r="B151" t="n">
-        <v>2.7</v>
+        <v>3.6</v>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>A reflected cross-site scripting vulnerability in the OAuth flow completion endpoints in Mattermost allows an attacker to send AJAX requests on behalf of the victim via sharing a crafted link with a malicious state parameter.</t>
+          <t>libcurl would reuse a previously created connection even when a TLS or SSHrelated option had been changed that should have prohibited reuse.libcurl keeps previously used connections in a connection pool for subsequenttransfers to reuse if one of them matches the setup. However, several TLS andSSH settings were left out from the configuration match checks, making themmatch too easily.</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>2023-03-21T15:26:57.867</t>
+          <t>2023-03-20T09:15:10.827</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>CVE-2023-1562</t>
-        </is>
-      </c>
-      <c r="B152" t="n">
-        <v>1.4</v>
-      </c>
+          <t>CVE-2023-0391</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr"/>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Mattermost fails to check the "Show Full Name" setting when rendering the result for the /plugins/focalboard/api/v2/users API call, allowing an attacker to learn the full name of a board owner.</t>
+          <t>MGT-COMMERCE CloudPanel ships with a static SSL certificate to encrypt communications to the administrative interface, shared across every installation of CloudPanel. This behavior was observed in version 2.2.0. There has been no indication from the vendor this has been addressed in version 2.2.1.</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>2023-03-22T12:47:56.330</t>
+          <t>2023-03-21T22:40:42.437</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>CVE-2023-22680</t>
+          <t>CVE-2023-28098</t>
         </is>
       </c>
       <c r="B153" t="n">
-        <v>2.7</v>
+        <v>3.6</v>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>Auth. (admin+) Stored Cross-Site Scripting (XSS) vulnerability in Altanic No API Amazon Affiliate plugin &lt;= 4.2.2 versions.</t>
+          <t>OpenSIPS is a Session Initiation Protocol (SIP) server implementation. Prior to versions 3.1.7 and 3.2.4, a specially crafted Authorization header causes OpenSIPS to crash or behave in an unexpected way due to a bug in the function `parse_param_name()` . This issue was discovered while performing coverage guided fuzzing of the function parse_msg. The AddressSanitizer identified that the issue occurred in the function `q_memchr()` which is being called by the function `parse_param_name()`. This issue may cause erratic program behaviour or a server crash. It affects configurations containing functions that make use of the affected code, such as the function `www_authorize()` . Versions 3.1.7 and 3.2.4 contain a fix.</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>2023-03-23T15:07:27.350</t>
+          <t>2023-03-21T22:39:28.990</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>CVE-2022-27782</t>
+          <t>CVE-2021-21548</t>
         </is>
       </c>
       <c r="B154" t="n">
-        <v>3.6</v>
+        <v>5.9</v>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>libcurl would reuse a previously created connection even when a TLS or SSHrelated option had been changed that should have prohibited reuse.libcurl keeps previously used connections in a connection pool for subsequenttransfers to reuse if one of them matches the setup. However, several TLS andSSH settings were left out from the configuration match checks, making themmatch too easily.</t>
+          <t>Dell EMC Unisphere for PowerMax versions before 9.1.0.27, Dell EMC Unisphere for PowerMax Virtual Appliance versions before 9.1.0.27, and PowerMax OS Release 5978 contain an improper certificate validation vulnerability. An unauthenticated remote attacker may potentially exploit this vulnerability to carry out a man-in-the-middle attack by supplying a crafted certificate and intercepting the victim's traffic to view or modify a victim’s data in transit.</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>2023-03-20T09:15:10.827</t>
+          <t>2023-03-17T12:59:31.617</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>CVE-2023-0361</t>
+          <t>CVE-2023-1570</t>
         </is>
       </c>
       <c r="B155" t="n">
-        <v>3.6</v>
+        <v>1.4</v>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>A timing side-channel in the handling of RSA ClientKeyExchange messages was discovered in GnuTLS. This side-channel can be sufficient to recover the key encrypted in the RSA ciphertext across a network in a Bleichenbacher style attack. To achieve a successful decryption the attacker would need to send a large amount of specially crafted messages to the vulnerable server. By recovering the secret from the ClientKeyExchange message, the attacker would be able to decrypt the application data exchanged over that connection.</t>
+          <t>A vulnerability, which was classified as problematic, has been found in syoyo tinydng. Affected by this issue is the function __interceptor_memcpy of the file tiny_dng_loader.h. The manipulation leads to heap-based buffer overflow. Local access is required to approach this attack. The exploit has been disclosed to the public and may be used. Continious delivery with rolling releases is used by this product. Therefore, no version details of affected nor updated releases are available. It is recommended to apply a patch to fix this issue. VDB-223562 is the identifier assigned to this vulnerability.</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>2023-03-18T07:15:10.870</t>
+          <t>2023-03-22T15:19:31.427</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>CVE-2023-28466</t>
-        </is>
-      </c>
-      <c r="B156" t="n">
-        <v>5.9</v>
-      </c>
+          <t>CVE-2023-27754</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr"/>
       <c r="C156" t="inlineStr">
         <is>
-          <t>do_tls_getsockopt in net/tls/tls_main.c in the Linux kernel through 6.2.6 lacks a lock_sock call, leading to a race condition (with a resultant use-after-free or NULL pointer dereference).</t>
+          <t>vox2mesh 1.0 has stack-overflow in main.cpp, this is stack-overflow caused by incorrect use of memcpy() funciton. The flow allows an attacker to cause a denial of service (abort) via a crafted file.</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>2023-03-21T17:27:19.377</t>
+          <t>2023-03-22T18:10:30.537</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>CVE-2023-0391</t>
-        </is>
-      </c>
-      <c r="B157" t="inlineStr"/>
+          <t>CVE-2023-27490</t>
+        </is>
+      </c>
+      <c r="B157" t="n">
+        <v>5.9</v>
+      </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>MGT-COMMERCE CloudPanel ships with a static SSL certificate to encrypt communications to the administrative interface, shared across every installation of CloudPanel. This behavior was observed in version 2.2.0. There has been no indication from the vendor this has been addressed in version 2.2.1.</t>
+          <t>NextAuth.js is an open source authentication solution for Next.js applications. `next-auth` applications using OAuth provider versions before `v4.20.1` have been found to be subject to an authentication vulnerability. A bad actor who can read traffic on the victim's network or who is able to social engineer the victim to click a manipulated login link could intercept and tamper with the authorization URL to **log in as the victim**, bypassing the CSRF protection. This is due to a partial failure during a compromised OAuth session where a session code is erroneously generated. This issue has been addressed in version 4.20.1. Users are advised to upgrade. Users unable to upgrade may using Advanced Initialization, manually check the callback request for state, pkce, and nonce against the provider configuration to prevent this issue. See the linked GHSA for details.</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>2023-03-21T22:40:42.437</t>
+          <t>2023-03-16T17:30:29.737</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>CVE-2023-28098</t>
-        </is>
-      </c>
-      <c r="B158" t="n">
-        <v>3.6</v>
-      </c>
+          <t>CVE-2022-3894</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr"/>
       <c r="C158" t="inlineStr">
         <is>
-          <t>OpenSIPS is a Session Initiation Protocol (SIP) server implementation. Prior to versions 3.1.7 and 3.2.4, a specially crafted Authorization header causes OpenSIPS to crash or behave in an unexpected way due to a bug in the function `parse_param_name()` . This issue was discovered while performing coverage guided fuzzing of the function parse_msg. The AddressSanitizer identified that the issue occurred in the function `q_memchr()` which is being called by the function `parse_param_name()`. This issue may cause erratic program behaviour or a server crash. It affects configurations containing functions that make use of the affected code, such as the function `www_authorize()` . Versions 3.1.7 and 3.2.4 contain a fix.</t>
+          <t>The WP OAuth Server (OAuth Authentication) WordPress plugin before 4.2.5 does not have CSRF check when deleting a client, and does not ensure that the object to be deleted is actually a client, which could allow attackers to make a logged in admin delete arbitrary client and post via a CSRF attack.</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>2023-03-21T22:39:28.990</t>
+          <t>2023-03-21T11:51:14.457</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>CVE-2021-21548</t>
-        </is>
-      </c>
-      <c r="B159" t="n">
-        <v>5.9</v>
-      </c>
+          <t>CVE-2022-4148</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr"/>
       <c r="C159" t="inlineStr">
         <is>
-          <t>Dell EMC Unisphere for PowerMax versions before 9.1.0.27, Dell EMC Unisphere for PowerMax Virtual Appliance versions before 9.1.0.27, and PowerMax OS Release 5978 contain an improper certificate validation vulnerability. An unauthenticated remote attacker may potentially exploit this vulnerability to carry out a man-in-the-middle attack by supplying a crafted certificate and intercepting the victim's traffic to view or modify a victim’s data in transit.</t>
+          <t>The WP OAuth Server (OAuth Authentication) WordPress plugin before 4.2.5 has a flawed CSRF and authorisation check when deleting a client, which could allow any authenticated users, such as subscriber to delete arbitrary client.</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>2023-03-17T12:59:31.617</t>
+          <t>2023-03-21T11:51:14.457</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>CVE-2023-1570</t>
+          <t>CVE-2023-1314</t>
         </is>
       </c>
       <c r="B160" t="n">
-        <v>1.4</v>
+        <v>5.8</v>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>A vulnerability, which was classified as problematic, has been found in syoyo tinydng. Affected by this issue is the function __interceptor_memcpy of the file tiny_dng_loader.h. The manipulation leads to heap-based buffer overflow. Local access is required to approach this attack. The exploit has been disclosed to the public and may be used. Continious delivery with rolling releases is used by this product. Therefore, no version details of affected nor updated releases are available. It is recommended to apply a patch to fix this issue. VDB-223562 is the identifier assigned to this vulnerability.</t>
+          <t>A vulnerability has been discovered in cloudflared's installer (&lt;= 2023.3.0) for Windows 32-bits devices that allows a local attacker with no administrative permissions to escalate their privileges on the affected device. This vulnerability exists because the MSI installer used by cloudflared relied on a world-writable directory. An attacker with local access to the device (without Administrator rights) can use symbolic links to trick the MSI installer into deleting files in locations that the attacker would otherwise have no access to. By creating a symlink from the world-writable directory to the target file, the attacker can manipulate the MSI installer's repair functionality to delete the target file during the repair process. Exploitation of this vulnerability could allow an attacker to delete important system files or replace them with malicious files, potentially leading to the affected device being compromised. The cloudflared client itself is not affected by this vulnerability, only the installer for 32-bit Windows devices.</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>2023-03-22T15:19:31.427</t>
+          <t>2023-03-21T12:19:40.680</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>CVE-2023-27754</t>
-        </is>
-      </c>
-      <c r="B161" t="inlineStr"/>
+          <t>CVE-2023-24859</t>
+        </is>
+      </c>
+      <c r="B161" t="n">
+        <v>3.6</v>
+      </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>vox2mesh 1.0 has stack-overflow in main.cpp, this is stack-overflow caused by incorrect use of memcpy() funciton. The flow allows an attacker to cause a denial of service (abort) via a crafted file.</t>
+          <t>Windows Internet Key Exchange (IKE) Extension Denial of Service Vulnerability</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>2023-03-22T18:10:30.537</t>
+          <t>2023-03-20T03:55:00.000</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>CVE-2023-27490</t>
+          <t>CVE-2023-23935</t>
         </is>
       </c>
       <c r="B162" t="n">
-        <v>5.9</v>
+        <v>1.4</v>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>NextAuth.js is an open source authentication solution for Next.js applications. `next-auth` applications using OAuth provider versions before `v4.20.1` have been found to be subject to an authentication vulnerability. A bad actor who can read traffic on the victim's network or who is able to social engineer the victim to click a manipulated login link could intercept and tamper with the authorization URL to **log in as the victim**, bypassing the CSRF protection. This is due to a partial failure during a compromised OAuth session where a session code is erroneously generated. This issue has been addressed in version 4.20.1. Users are advised to upgrade. Users unable to upgrade may using Advanced Initialization, manually check the callback request for state, pkce, and nonce against the provider configuration to prevent this issue. See the linked GHSA for details.</t>
+          <t>Discourse is an open-source messaging platform. In versions 3.0.1 and prior on the `stable` branch and versions 3.1.0.beta2 and prior on the `beta` and `tests-passed` branches, the count of personal messages displayed for a tag is a count of all personal messages regardless of whether the personal message is visible to a given user. As a result, any users can technically poll a sensitive tag to determine if a new personal message is created even if the user does not have access to the personal message. In the patched versions, the count of personal messages tagged with a given tag is hidden by default. To revert to the old behaviour of displaying the count of personal messages for a given tag, an admin may enable the `display_personal_messages_tag_counts` site setting.</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>2023-03-16T17:30:29.737</t>
+          <t>2023-03-23T14:57:04.963</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>CVE-2022-3894</t>
-        </is>
-      </c>
-      <c r="B163" t="inlineStr"/>
+          <t>CVE-2023-23622</t>
+        </is>
+      </c>
+      <c r="B163" t="n">
+        <v>1.4</v>
+      </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>The WP OAuth Server (OAuth Authentication) WordPress plugin before 4.2.5 does not have CSRF check when deleting a client, and does not ensure that the object to be deleted is actually a client, which could allow attackers to make a logged in admin delete arbitrary client and post via a CSRF attack.</t>
+          <t>Discourse is an open-source discussion platform. Prior to version 3.0.1 of the `stable` branch and version 3.1.0.beta2 of the `beta` and `tests-passed` branches, the count of topics displayed for a tag is a count of all regular topics regardless of whether the topic is in a read restricted category or not. As a result, any users can technically poll a sensitive tag to determine if a new topic is created in a category which the user does not have excess to. In version 3.0.1 of the `stable` branch and version 3.1.0.beta2 of the `beta` and `tests-passed` branches, the count of topics displayed for a tag defaults to only counting regular topics which are not in read restricted categories. Staff users will continue to see a count of all topics regardless of the topic's category read restrictions.</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>2023-03-21T11:51:14.457</t>
+          <t>2023-03-17T15:44:01.930</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>CVE-2022-4148</t>
-        </is>
-      </c>
-      <c r="B164" t="inlineStr"/>
+          <t>CVE-2023-26040</t>
+        </is>
+      </c>
+      <c r="B164" t="n">
+        <v>2.5</v>
+      </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>The WP OAuth Server (OAuth Authentication) WordPress plugin before 4.2.5 has a flawed CSRF and authorisation check when deleting a client, which could allow any authenticated users, such as subscriber to delete arbitrary client.</t>
+          <t>Discourse is an open-source discussion platform. Between versions 3.1.0.beta2 and 3.1.0.beta3 of the `tests-passed` branch, editing or responding to a chat message containing malicious content could lead to a cross-site scripting attack. This issue is patched in version 3.1.0.beta3 of the `tests-passed` branch. There are no known workarounds.</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>2023-03-21T11:51:14.457</t>
+          <t>2023-03-17T15:44:01.930</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>CVE-2023-1314</t>
+          <t>CVE-2023-25172</t>
         </is>
       </c>
       <c r="B165" t="n">
-        <v>5.8</v>
+        <v>2.7</v>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>A vulnerability has been discovered in cloudflared's installer (&lt;= 2023.3.0) for Windows 32-bits devices that allows a local attacker with no administrative permissions to escalate their privileges on the affected device. This vulnerability exists because the MSI installer used by cloudflared relied on a world-writable directory. An attacker with local access to the device (without Administrator rights) can use symbolic links to trick the MSI installer into deleting files in locations that the attacker would otherwise have no access to. By creating a symlink from the world-writable directory to the target file, the attacker can manipulate the MSI installer's repair functionality to delete the target file during the repair process. Exploitation of this vulnerability could allow an attacker to delete important system files or replace them with malicious files, potentially leading to the affected device being compromised. The cloudflared client itself is not affected by this vulnerability, only the installer for 32-bit Windows devices.</t>
+          <t>Discourse is an open-source discussion platform. Prior to version 3.0.1 of the `stable` branch and version 3.1.0.beta2 of the `beta` and `tests-passed` branches, a maliciously crafted URL can be included in a user's full name field to to carry out cross-site scripting attacks on sites with a disabled or overly permissive CSP (Content Security Policy). Discourse's default CSP prevents this vulnerability. The vulnerability is patched in version 3.0.1 of the `stable` branch and version 3.1.0.beta2 of the `beta` and `tests-passed` branches. As a workaround, enable and/or restore your site's CSP to the default one provided with Discourse.</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>2023-03-21T12:19:40.680</t>
+          <t>2023-03-20T02:46:58.537</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>CVE-2023-24859</t>
+          <t>CVE-2023-28107</t>
         </is>
       </c>
       <c r="B166" t="n">
@@ -3714,119 +3714,119 @@
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>Windows Internet Key Exchange (IKE) Extension Denial of Service Vulnerability</t>
+          <t>Discourse is an open-source discussion platform. Prior to version 3.0.2 of the `stable` branch and version 3.1.0.beta3 of the `beta` and `tests-passed` branches, a user logged as an administrator can request backups multiple times, which will eat up all the connections to the DB. If this is done on a site using multisite, then it can affect the whole cluster. The vulnerability is patched in version 3.0.2 of the `stable` branch and version 3.1.0.beta3 of the `beta` and `tests-passed` branches. There are no known workarounds.</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>2023-03-20T03:55:00.000</t>
+          <t>2023-03-20T02:46:58.537</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>CVE-2023-23935</t>
+          <t>CVE-2018-7084</t>
         </is>
       </c>
       <c r="B167" t="n">
-        <v>1.4</v>
+        <v>5.9</v>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>Discourse is an open-source messaging platform. In versions 3.0.1 and prior on the `stable` branch and versions 3.1.0.beta2 and prior on the `beta` and `tests-passed` branches, the count of personal messages displayed for a tag is a count of all personal messages regardless of whether the personal message is visible to a given user. As a result, any users can technically poll a sensitive tag to determine if a new personal message is created even if the user does not have access to the personal message. In the patched versions, the count of personal messages tagged with a given tag is hidden by default. To revert to the old behaviour of displaying the count of personal messages for a given tag, an admin may enable the `display_personal_messages_tag_counts` site setting.</t>
+          <t>A command injection vulnerability is present that permits an unauthenticated user with access to the Aruba Instant web interface to execute arbitrary system commands within the underlying operating system. An attacker could use this ability to copy files, read configuration, write files, delete files, or reboot the device. Workaround: Block access to the Aruba Instant web interface from all untrusted users. Resolution: Fixed in Aruba Instant 4.2.4.12, 6.5.4.11, 8.3.0.6, and 8.4.0.1</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>2023-03-23T14:57:04.963</t>
+          <t>2023-03-20T18:11:53.287</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>CVE-2023-23622</t>
+          <t>CVE-2023-1168</t>
         </is>
       </c>
       <c r="B168" t="n">
-        <v>1.4</v>
+        <v>5.9</v>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>Discourse is an open-source discussion platform. Prior to version 3.0.1 of the `stable` branch and version 3.1.0.beta2 of the `beta` and `tests-passed` branches, the count of topics displayed for a tag is a count of all regular topics regardless of whether the topic is in a read restricted category or not. As a result, any users can technically poll a sensitive tag to determine if a new topic is created in a category which the user does not have excess to. In version 3.0.1 of the `stable` branch and version 3.1.0.beta2 of the `beta` and `tests-passed` branches, the count of topics displayed for a tag defaults to only counting regular topics which are not in read restricted categories. Staff users will continue to see a count of all topics regardless of the topic's category read restrictions.</t>
+          <t>An authenticated remote code execution vulnerability exists in the AOS-CX Network Analytics Engine. Successful exploitation of this vulnerability results in the ability to execute arbitrary code as a privileged user on the underlying operating system, leading to a complete compromise of the switch running AOS-CX.</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>2023-03-17T15:44:01.930</t>
+          <t>2023-03-22T12:48:04.240</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>CVE-2023-26040</t>
+          <t>CVE-2023-25589</t>
         </is>
       </c>
       <c r="B169" t="n">
-        <v>2.5</v>
+        <v>5.9</v>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>Discourse is an open-source discussion platform. Between versions 3.1.0.beta2 and 3.1.0.beta3 of the `tests-passed` branch, editing or responding to a chat message containing malicious content could lead to a cross-site scripting attack. This issue is patched in version 3.1.0.beta3 of the `tests-passed` branch. There are no known workarounds.</t>
+          <t>A vulnerability in the web-based management interface of ClearPass Policy Manager could allow an unauthenticated remote attacker to create arbitrary users on the platform. A successful exploit allows an attacker to achieve total cluster compromise.</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>2023-03-17T15:44:01.930</t>
+          <t>2023-03-22T12:48:04.240</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>CVE-2023-25172</t>
+          <t>CVE-2023-25590</t>
         </is>
       </c>
       <c r="B170" t="n">
-        <v>2.7</v>
+        <v>5.9</v>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>Discourse is an open-source discussion platform. Prior to version 3.0.1 of the `stable` branch and version 3.1.0.beta2 of the `beta` and `tests-passed` branches, a maliciously crafted URL can be included in a user's full name field to to carry out cross-site scripting attacks on sites with a disabled or overly permissive CSP (Content Security Policy). Discourse's default CSP prevents this vulnerability. The vulnerability is patched in version 3.0.1 of the `stable` branch and version 3.1.0.beta2 of the `beta` and `tests-passed` branches. As a workaround, enable and/or restore your site's CSP to the default one provided with Discourse.</t>
+          <t>A vulnerability in the ClearPass OnGuard Linux agent could allow malicious users on a Linux instance to elevate their user privileges to those of a higher role. A successful exploit allows malicious users to execute arbitrary code with root level privileges on the Linux instance.</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>2023-03-20T02:46:58.537</t>
+          <t>2023-03-22T12:47:56.330</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>CVE-2023-28107</t>
+          <t>CVE-2023-25591</t>
         </is>
       </c>
       <c r="B171" t="n">
-        <v>3.6</v>
+        <v>4.7</v>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>Discourse is an open-source discussion platform. Prior to version 3.0.2 of the `stable` branch and version 3.1.0.beta3 of the `beta` and `tests-passed` branches, a user logged as an administrator can request backups multiple times, which will eat up all the connections to the DB. If this is done on a site using multisite, then it can affect the whole cluster. The vulnerability is patched in version 3.0.2 of the `stable` branch and version 3.1.0.beta3 of the `beta` and `tests-passed` branches. There are no known workarounds.</t>
+          <t>A vulnerability in the web-based management interface of ClearPass Policy Manager could allow a remote attacker authenticated with low privileges to access sensitive information. A successful exploit allows an attacker to retrieve information which could be used to potentially gain further privileges on the ClearPass instance.</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>2023-03-20T02:46:58.537</t>
+          <t>2023-03-22T12:47:56.330</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>CVE-2018-7084</t>
+          <t>CVE-2022-47629</t>
         </is>
       </c>
       <c r="B172" t="n">
@@ -3834,19 +3834,19 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>A command injection vulnerability is present that permits an unauthenticated user with access to the Aruba Instant web interface to execute arbitrary system commands within the underlying operating system. An attacker could use this ability to copy files, read configuration, write files, delete files, or reboot the device. Workaround: Block access to the Aruba Instant web interface from all untrusted users. Resolution: Fixed in Aruba Instant 4.2.4.12, 6.5.4.11, 8.3.0.6, and 8.4.0.1</t>
+          <t>Libksba before 1.6.3 is prone to an integer overflow vulnerability in the CRL signature parser.</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>2023-03-20T18:11:53.287</t>
+          <t>2023-03-16T21:15:11.357</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>CVE-2023-1168</t>
+          <t>CVE-2023-24468</t>
         </is>
       </c>
       <c r="B173" t="n">
@@ -3854,19 +3854,19 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>An authenticated remote code execution vulnerability exists in the AOS-CX Network Analytics Engine. Successful exploitation of this vulnerability results in the ability to execute arbitrary code as a privileged user on the underlying operating system, leading to a complete compromise of the switch running AOS-CX.</t>
+          <t>Broken access control in Advanced Authentication versions prior to 6.4.1.1 and 6.3.7.2</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>2023-03-22T12:48:04.240</t>
+          <t>2023-03-19T03:47:27.013</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>CVE-2023-25589</t>
+          <t>CVE-2023-28434</t>
         </is>
       </c>
       <c r="B174" t="n">
@@ -3874,110 +3874,10 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>A vulnerability in the web-based management interface of ClearPass Policy Manager could allow an unauthenticated remote attacker to create arbitrary users on the platform. A successful exploit allows an attacker to achieve total cluster compromise.</t>
+          <t>Minio is a Multi-Cloud Object Storage framework. Prior to RELEASE.2023-03-20T20-16-18Z, an attacker can use crafted requests to bypass metadata bucket name checking and put an object into any bucket while processing `PostPolicyBucket`. To carry out this attack, the attacker requires credentials with `arn:aws:s3:::*` permission, as well as enabled Console API access. This issue has been patched in RELEASE.2023-03-20T20-16-18Z. As a workaround, enable browser API access and turn off `MINIO_BROWSER=off`.</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
-        <is>
-          <t>2023-03-22T12:48:04.240</t>
-        </is>
-      </c>
-    </row>
-    <row r="175">
-      <c r="A175" t="inlineStr">
-        <is>
-          <t>CVE-2023-25590</t>
-        </is>
-      </c>
-      <c r="B175" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="C175" t="inlineStr">
-        <is>
-          <t>A vulnerability in the ClearPass OnGuard Linux agent could allow malicious users on a Linux instance to elevate their user privileges to those of a higher role. A successful exploit allows malicious users to execute arbitrary code with root level privileges on the Linux instance.</t>
-        </is>
-      </c>
-      <c r="D175" t="inlineStr">
-        <is>
-          <t>2023-03-22T12:47:56.330</t>
-        </is>
-      </c>
-    </row>
-    <row r="176">
-      <c r="A176" t="inlineStr">
-        <is>
-          <t>CVE-2023-25591</t>
-        </is>
-      </c>
-      <c r="B176" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="C176" t="inlineStr">
-        <is>
-          <t>A vulnerability in the web-based management interface of ClearPass Policy Manager could allow a remote attacker authenticated with low privileges to access sensitive information. A successful exploit allows an attacker to retrieve information which could be used to potentially gain further privileges on the ClearPass instance.</t>
-        </is>
-      </c>
-      <c r="D176" t="inlineStr">
-        <is>
-          <t>2023-03-22T12:47:56.330</t>
-        </is>
-      </c>
-    </row>
-    <row r="177">
-      <c r="A177" t="inlineStr">
-        <is>
-          <t>CVE-2022-47629</t>
-        </is>
-      </c>
-      <c r="B177" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="C177" t="inlineStr">
-        <is>
-          <t>Libksba before 1.6.3 is prone to an integer overflow vulnerability in the CRL signature parser.</t>
-        </is>
-      </c>
-      <c r="D177" t="inlineStr">
-        <is>
-          <t>2023-03-16T21:15:11.357</t>
-        </is>
-      </c>
-    </row>
-    <row r="178">
-      <c r="A178" t="inlineStr">
-        <is>
-          <t>CVE-2023-24468</t>
-        </is>
-      </c>
-      <c r="B178" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="C178" t="inlineStr">
-        <is>
-          <t>Broken access control in Advanced Authentication versions prior to 6.4.1.1 and 6.3.7.2</t>
-        </is>
-      </c>
-      <c r="D178" t="inlineStr">
-        <is>
-          <t>2023-03-19T03:47:27.013</t>
-        </is>
-      </c>
-    </row>
-    <row r="179">
-      <c r="A179" t="inlineStr">
-        <is>
-          <t>CVE-2023-28434</t>
-        </is>
-      </c>
-      <c r="B179" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="C179" t="inlineStr">
-        <is>
-          <t>Minio is a Multi-Cloud Object Storage framework. Prior to RELEASE.2023-03-20T20-16-18Z, an attacker can use crafted requests to bypass metadata bucket name checking and put an object into any bucket while processing `PostPolicyBucket`. To carry out this attack, the attacker requires credentials with `arn:aws:s3:::*` permission, as well as enabled Console API access. This issue has been patched in RELEASE.2023-03-20T20-16-18Z. As a workaround, enable browser API access and turn off `MINIO_BROWSER=off`.</t>
-        </is>
-      </c>
-      <c r="D179" t="inlineStr">
         <is>
           <t>2023-03-23T01:02:56.037</t>
         </is>

</xml_diff>

<commit_message>
adding link column and encoding, works for windows but does the bot...
</commit_message>
<xml_diff>
--- a/cves.xlsx
+++ b/cves.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,300 +459,365 @@
           <t>Last Modified</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>CVE-2021-3293</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>1.4</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>PHP</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>emlog v5.3.1 has full path disclosure vulnerability in t/index.php, which allows an attacker to see the path to the webroot/file.</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>2023-03-20T20:31:47.667</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>https://cve.circl.lu/cve/CVE-2021-3293</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CVE-2020-28871</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>5.9</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>PHP</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Remote code execution in Monitorr v1.7.6m in upload.php allows an unauthorized person to execute arbitrary code on the server-side via an insecure file upload.</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>2023-03-23T17:15:13.497</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>https://cve.circl.lu/cve/CVE-2020-28871</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CVE-2022-44355</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>2.7</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>PHP</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>SolarView Compact 7.0 is vulnerable to Cross-site Scripting (XSS) via /network_test.php.</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>2023-03-23T17:17:48.153</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>https://cve.circl.lu/cve/CVE-2022-44355</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>CVE-2023-27478</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>2.5</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>PHP</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>libmemcached-awesome is an open source C/C++ client library and tools for the memcached server. `libmemcached` could return data for a previously requested key, if that previous request timed out due to a low `POLL_TIMEOUT`. This issue has been addressed in version 1.1.4. Users are advised to upgrade. There are several ways to workaround or lower the probability of this bug affecting a given deployment. 1: use a reasonably high `POLL_TIMEOUT` setting, like the default. 2: use separate libmemcached connections for unrelated data. 3: do not re-use libmemcached connections in an unknown state.</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>2023-03-23T16:59:14.237</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>https://cve.circl.lu/cve/CVE-2023-27478</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>CVE-2023-27580</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>3.6</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>PHP</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>CodeIgniter Shield provides authentication and authorization for the CodeIgniter 4 PHP framework. An improper implementation was found in the password storage process. All hashed passwords stored in Shield v1.0.0-beta.3 or earlier are easier to crack than expected due to the vulnerability. Therefore, they should be removed as soon as possible. If an attacker gets (1) the user's hashed password by Shield, and (2) the hashed password (SHA-384 hash without salt) from somewhere, the attacker may easily crack the user's password. Upgrade to Shield v1.0.0-beta.4 or later to fix this issue. After upgrading, all users’ hashed passwords should be updated (saved to the database). There are no known workarounds.</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>2023-03-23T15:13:04.287</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>https://cve.circl.lu/cve/CVE-2023-27580</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>CVE-2023-28725</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
         <is>
           <t>Bitcoin</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>General Bytes Crypto Application Server (CAS) 20230120, as distributed with General Bytes BATM devices, allows remote attackers to execute arbitrary Java code by uploading a Java application to the /batm/app/admin/standalone/deployments directory, aka BATM-4780, as exploited in the wild in March 2023. This is fixed in 20221118.48 and 20230120.44.</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>2023-03-22T12:48:04.240</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>https://cve.circl.lu/cve/CVE-2023-28725</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>CVE-2022-47145</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>3.7</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>Bitcoin</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>Reflected Cross-Site Scripting (XSS) vulnerability in Blockonomics WordPress Bitcoin Payments – Blockonomics plugin &lt;= 3.5.7 versions.</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>2023-03-24T01:57:07.650</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>https://cve.circl.lu/cve/CVE-2022-47145</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>CVE-2023-24571</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
         <v>5.9</v>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>Dell</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>Dell BIOS contains an Improper Input Validation vulnerability. A local authenticated malicious user with administrator privileges could potentially exploit this vulnerability to perform arbitrary code execution.</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>2023-03-21T22:30:08.107</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>https://cve.circl.lu/cve/CVE-2023-24571</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>CVE-2022-34406</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
         <v>5.9</v>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>Dell</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>Dell PowerEdge BIOS and Dell Precision BIOS contain an Improper SMM communication buffer verification vulnerability. A local malicious user with high Privileges may potentially exploit this vulnerability to perform arbitrary code execution or cause denial of service.</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>2023-03-22T17:20:57.133</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>https://cve.circl.lu/cve/CVE-2022-34406</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>CVE-2022-34407</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
         <v>5.9</v>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>Dell</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>Dell PowerEdge BIOS and Dell Precision BIOS contain an Improper SMM communication buffer verification vulnerability. A local malicious user with high Privileges may potentially exploit this vulnerability to perform arbitrary code execution or cause denial of service.</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>2023-03-22T17:21:28.703</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>https://cve.circl.lu/cve/CVE-2022-34407</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>CVE-2022-34408</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
         <v>5.9</v>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>Dell</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>Dell PowerEdge BIOS and Dell Precision BIOS contain an Improper SMM communication buffer verification vulnerability. A local malicious user with high Privileges may potentially exploit this vulnerability to perform arbitrary code execution or cause denial of service.</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>2023-03-24T14:53:26.990</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>https://cve.circl.lu/cve/CVE-2022-34408</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>CVE-2022-34409</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
         <v>5.9</v>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>Dell</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>Dell PowerEdge BIOS and Dell Precision BIOS contain an Improper SMM communication buffer verification vulnerability. A local malicious user with high Privileges may potentially exploit this vulnerability to perform arbitrary code execution or cause denial of service.</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>2023-03-22T14:49:27.497</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>https://cve.circl.lu/cve/CVE-2022-34409</t>
         </is>

</xml_diff>